<commit_message>
fixes test output issue
</commit_message>
<xml_diff>
--- a/temp/test.xlsx
+++ b/temp/test.xlsx
@@ -29,12 +29,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>jonsmith</t>
   </si>
   <si>
@@ -42,6 +36,12 @@
   </si>
   <si>
     <t>Smith</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,21 +369,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removes some previous changes and adds null type fix
Data must be JSON serializable.
</commit_message>
<xml_diff>
--- a/temp/test.xlsx
+++ b/temp/test.xlsx
@@ -26,22 +26,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>jonsmith</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>jon1234</t>
   </si>
 </sst>
 </file>
@@ -359,31 +359,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>